<commit_message>
fix(publipostage): Refactor synthetic array /3
</commit_message>
<xml_diff>
--- a/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
+++ b/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
@@ -55,22 +55,22 @@
     <t>intervention_type</t>
   </si>
   <si>
-    <t>🟥</t>
-  </si>
-  <si>
-    <t>⬛</t>
-  </si>
-  <si>
-    <t>🟧</t>
-  </si>
-  <si>
-    <t>🟩</t>
+    <t>📕</t>
+  </si>
+  <si>
+    <t>📘</t>
+  </si>
+  <si>
+    <t>📙</t>
+  </si>
+  <si>
+    <t>📗</t>
   </si>
   <si>
     <t>rouge</t>
   </si>
   <si>
-    <t>noir</t>
+    <t>bleu</t>
   </si>
   <si>
     <t>orange</t>

</xml_diff>

<commit_message>
fix(publipostage): Try to solve Excel emoji problem
</commit_message>
<xml_diff>
--- a/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
+++ b/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
@@ -55,16 +55,16 @@
     <t>intervention_type</t>
   </si>
   <si>
-    <t>📕</t>
-  </si>
-  <si>
-    <t>📘</t>
-  </si>
-  <si>
-    <t>📙</t>
-  </si>
-  <si>
-    <t>📗</t>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>⚠️</t>
+  </si>
+  <si>
+    <t>+3</t>
+  </si>
+  <si>
+    <t>✅</t>
   </si>
   <si>
     <t>rouge</t>

</xml_diff>

<commit_message>
fix(publipostage): Correct status name
</commit_message>
<xml_diff>
--- a/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
+++ b/publipostage2/002cp4060/liste_essais_cliniques_identifies_002cp4060.xlsx
@@ -70,7 +70,7 @@
     <t>rouge</t>
   </si>
   <si>
-    <t>bleu</t>
+    <t>noir</t>
   </si>
   <si>
     <t>orange</t>
@@ -79,16 +79,16 @@
     <t>vert</t>
   </si>
   <si>
-    <t>résultat et / ou publication posté</t>
-  </si>
-  <si>
-    <t>pas de résultat ni de publication</t>
-  </si>
-  <si>
-    <t>résultat et / ou publication posté dans les 36 mois</t>
-  </si>
-  <si>
-    <t>résultat et / ou publication posté dans les 12 mois</t>
+    <t>résultat postés ou publiés</t>
+  </si>
+  <si>
+    <t>pas de résultat postés ni publiés</t>
+  </si>
+  <si>
+    <t>résultat postés ou publiés dans les 36 mois</t>
+  </si>
+  <si>
+    <t>résultat postés ou publiés dans les 12 mois</t>
   </si>
   <si>
     <t>NCT00299650</t>

</xml_diff>